<commit_message>
Mise à jour du format du fichier tra des R3A.
</commit_message>
<xml_diff>
--- a/formats/excel/PSY/tra/Formats TRA PSY_R3A xx.xlsx
+++ b/formats/excel/PSY/tra/Formats TRA PSY_R3A xx.xlsx
@@ -1,22 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3021771\Documents\Ressources\R\Methods\formats_pmeasyr\formats\excel\PSY\tra\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0211E82-2760-4EC6-8ADE-E96B2FA73B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="405" windowWidth="23475" windowHeight="10515"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>nom</t>
   </si>
@@ -91,12 +108,18 @@
   </si>
   <si>
     <t>Lieu de l'acte</t>
+  </si>
+  <si>
+    <t>MODREALACT</t>
+  </si>
+  <si>
+    <t>Modalité de réalisation de l'acte</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -145,6 +168,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -192,7 +218,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -225,9 +251,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -260,6 +303,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -435,10 +495,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -447,7 +509,7 @@
     <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -535,13 +597,13 @@
         <v>13</v>
       </c>
       <c r="B5" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2">
         <v>37</v>
       </c>
       <c r="D5" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>7</v>
@@ -558,10 +620,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="2">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D6" s="2">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>7</v>
@@ -578,10 +640,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="2">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D7" s="2">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>7</v>
@@ -598,10 +660,10 @@
         <v>8</v>
       </c>
       <c r="C8" s="2">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D8" s="2">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>7</v>
@@ -615,13 +677,13 @@
         <v>21</v>
       </c>
       <c r="B9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="2">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D9" s="2">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>7</v>
@@ -638,16 +700,36 @@
         <v>3</v>
       </c>
       <c r="C10" s="2">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D10" s="2">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>59</v>
+      </c>
+      <c r="D11" s="2">
+        <v>59</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -656,7 +738,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -668,7 +750,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>